<commit_message>
cn-#17 Implementing Background Feature
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/SampleConversion.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/SampleConversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B058F6BC-B7FC-4482-A28C-FC3C985569BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CB1A8A-0AE5-422A-936A-17E61EFE5DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Conversion" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Given</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>"../../../../Cactus.ReqnrollVerificationTest/Features"</t>
+  </si>
+  <si>
+    <t>Background Sample Conversion</t>
+  </si>
+  <si>
+    <t>BackgroundSample.xlsx</t>
   </si>
 </sst>
 </file>
@@ -137,9 +143,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D12"/>
+  <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E12"/>
+      <selection activeCell="D12" sqref="D12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +474,7 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -534,6 +539,18 @@
       <c r="D12" t="str">
         <f>SUBSTITUTE(C12, ".xlsx", ".ExpectedFeature")</f>
         <v>ScenarioOutlineSample.ExpectedFeature</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="str">
+        <f>SUBSTITUTE(C13, ".xlsx", ".ExpectedFeature")</f>
+        <v>BackgroundSample.ExpectedFeature</v>
       </c>
     </row>
   </sheetData>

</xml_diff>